<commit_message>
Add item structures, Add item file reader, Add Send itemVersion when loginResponse
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -537,7 +537,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>s / f</t>
+    <t>[item version] / f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -944,7 +944,7 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add timer for each room, Add gameStart (message model, logic)
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire\TheVampire_Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -546,13 +546,21 @@
   </si>
   <si>
     <t>s [ public / pricvate]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game start (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -952,7 +960,7 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1337,10 +1345,14 @@
       <c r="E18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>

</xml_diff>

<commit_message>
Add Games.cs(SetClass), Modify PlayerInfo
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\TheVampire_Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,7 +553,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;empty&gt;</t>
+    <t>v / h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Add message model(randomNumber, cardSubmit, gameInfo) and random response processing, Add Player states
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\TheVampire_Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire\TheVampire_Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="142">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -269,46 +269,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>107</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>114</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>116</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>122(z)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -405,10 +365,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[infomation of server]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -554,6 +510,90 @@
   </si>
   <si>
     <t>v / h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random number R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107(k)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random number (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[long number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number: 0 ~ 999,999,999,999,999</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>card submit R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[cardNo] &lt;[targetID]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game battle info (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>108(l)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109(m)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110(n)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111(o)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>112(p)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113(q)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>114(r)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>116(t)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>117(u)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[targetID] [class] / [message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[targetID] [hp]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -959,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -970,9 +1010,10 @@
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.75" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="1.25" customWidth="1"/>
-    <col min="8" max="9" width="30.625" customWidth="1"/>
+    <col min="8" max="8" width="30.625" customWidth="1"/>
+    <col min="9" max="9" width="33.625" customWidth="1"/>
     <col min="10" max="10" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1051,7 +1092,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1070,17 +1111,17 @@
         <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -1100,13 +1141,13 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="K7" s="3"/>
     </row>
@@ -1122,7 +1163,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
@@ -1144,14 +1185,14 @@
         <v>40</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1180,21 +1221,21 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="K11" s="3"/>
     </row>
@@ -1214,13 +1255,13 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K12" s="3"/>
     </row>
@@ -1234,11 +1275,11 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1250,20 +1291,20 @@
         <v>54</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1274,20 +1315,20 @@
         <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1298,23 +1339,23 @@
         <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="K16" s="3"/>
     </row>
@@ -1324,34 +1365,29 @@
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1359,59 +1395,78 @@
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="E19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1423,11 +1478,11 @@
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1439,11 +1494,11 @@
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1455,11 +1510,11 @@
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1471,11 +1526,11 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1487,67 +1542,44 @@
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>123</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1555,105 +1587,112 @@
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="E31" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="I31" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="C32" s="3" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="3" t="s">
+      <c r="I34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="3" t="s">
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>

</xml_diff>

<commit_message>
Add Ack&Retransfer proc, Disable roomIn&Out(errors)
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="151">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -345,267 +345,291 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>\r\n: separator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s [room info] / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f: room unabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88(X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[infomation of server]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>89(Y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>89(Z)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>by admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[notice type] [message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[sender]\r\n[message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monitor R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a(ll) / c(lients) / r(ooms) / e(rrors)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[room number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>by admin, $sep$: separator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121(y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>119(w)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[friend id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail to room enter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[public room info list]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lobbyNum totalNum maximumNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lobby info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[item version] / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disconnect R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>118(v)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item list R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[item list]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[isPublic]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s [t / f] / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s [ public / pricvate]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game start (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v / h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random number R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107(k)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random number (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[long number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number: 0 ~ 999,999,999,999,999</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>card submit R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[cardNo] &lt;[targetID]&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>108(l)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109(m)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110(n)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111(o)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>112(p)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113(q)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>114(r)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>116(t)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>117(u)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room in/out (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i/o [userID]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timer update (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[timer]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[turn] [[targetID] [hp]]*4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game turn info (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>serial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ack R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>notice</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>\r\n: separator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s [room info] / f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f: room unabled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88(X)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[infomation of server]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89(Y)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89(Z)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>120(x)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notice R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by admin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[notice type] [message]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[message]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[sender]\r\n[message]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monitor R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>monitor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a(ll) / c(lients) / r(ooms) / e(rrors)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[room number]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>by admin, $sep$: separator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>121(y)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>119(w)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[friend id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail to room enter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[public room info list]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lobbyNum totalNum maximumNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lobby info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[101]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[item version] / f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>disconnect R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>118(v)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>item list R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>item list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[item list]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[isPublic]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s [t / f] / f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s [ public / pricvate]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>game start (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v / h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>random number R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>107(k)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>random number (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[long number]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number: 0 ~ 999,999,999,999,999</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>card submit R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[cardNo] &lt;[targetID]&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>game info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>108(l)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>109(m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110(n)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111(o)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>112(p)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>113(q)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>114(r)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>115(s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>116(t)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>117(u)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room in/out (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i/o [userID]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timer update (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[timer]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[turn] [[targetID] [hp]]*4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>game turn info (multicast)</t>
+    <t>[ackSerial] / &lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>empty: retransfer Request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X(server)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$s$[serial]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1009,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K37"/>
+  <dimension ref="B1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1128,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1123,17 +1147,17 @@
         <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -1153,13 +1177,13 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="K7" s="3"/>
     </row>
@@ -1175,7 +1199,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
@@ -1197,14 +1221,14 @@
         <v>40</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1244,10 +1268,10 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="K11" s="3"/>
     </row>
@@ -1267,13 +1291,13 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="J12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" s="3"/>
     </row>
@@ -1291,7 +1315,7 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1361,7 +1385,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>77</v>
@@ -1394,12 +1418,12 @@
         <v>59</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1410,20 +1434,20 @@
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="G19" s="3"/>
       <c r="I19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="K19" s="3"/>
     </row>
@@ -1433,20 +1457,20 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1458,35 +1482,37 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1498,15 +1524,15 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1518,7 +1544,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1534,7 +1560,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1550,7 +1576,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1561,12 +1587,8 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1576,7 +1598,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1586,7 +1608,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E29" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1595,13 +1617,24 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="E30" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="J30" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
@@ -1610,44 +1643,44 @@
         <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="3"/>
       <c r="G33" s="3"/>
@@ -1656,51 +1689,51 @@
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
@@ -1718,6 +1751,14 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Modify something(socket transfer), Add dataStack processing
</commit_message>
<xml_diff>
--- a/message model.xlsx
+++ b/message model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="158">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -642,6 +642,22 @@
   </si>
   <si>
     <t>v / h: winner's team, d: draw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>game info + turn info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[message]\r\n[turn] [[targetID] [hp]]*4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n\r: separator</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1045,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K38"/>
+  <dimension ref="B1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1061,7 +1077,7 @@
     <col min="6" max="6" width="24.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="1.25" customWidth="1"/>
     <col min="8" max="8" width="30.625" customWidth="1"/>
-    <col min="9" max="9" width="33.625" customWidth="1"/>
+    <col min="9" max="9" width="35" customWidth="1"/>
     <col min="10" max="10" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1174,7 +1190,9 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1628,13 +1646,22 @@
       <c r="E29" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="G29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C30" s="3" t="s">
         <v>19</v>
       </c>
@@ -1777,6 +1804,23 @@
       <c r="F38" s="1" t="s">
         <v>150</v>
       </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>